<commit_message>
Feature: Actions ahora chequea precios de polygon y envía mensajes al bot de Telegram
</commit_message>
<xml_diff>
--- a/actions.xlsx
+++ b/actions.xlsx
@@ -7,9 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 empresas del momento" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 acciones bajas" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Totales" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Totales" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acciones invertidas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 empresas del momento" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 acciones bajas" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,6 +416,42 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -461,42 +498,42 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Facebook</t>
+          <t>Google</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Alphabet</t>
+          <t>Alibaba</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Shopify</t>
+          <t>Facebook</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Netflix</t>
+          <t>Berkshire Hathaway</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Square</t>
+          <t>Johnson &amp; Johnson</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Stay diversified with your investments</t>
+          <t>Diversify your portfolio</t>
         </is>
       </c>
     </row>
@@ -505,7 +542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -529,70 +566,70 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nokia</t>
+          <t>PennyMac Financial Services</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BlackBerry</t>
+          <t>Amkor Technology</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GameStop</t>
+          <t>Air Lease Corporation</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AMC Entertainment</t>
+          <t>Baozun</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Koss Corporation</t>
+          <t>Qurate Retail</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Express</t>
+          <t>Guess</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Naked Brand Group</t>
+          <t>UniFirst</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Sundial Growers</t>
+          <t>Commvault Systems</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ebang International</t>
+          <t>Prudental Financial</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Invest wisely, don't pour all your capital into a single economic sector. Diversification is important.</t>
+          <t>Understanding and using eToro's CopyTrader feature wisely</t>
         </is>
       </c>
     </row>
@@ -606,92 +643,74 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Nokia</t>
+          <t>PennyMac Financial Services</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BlackBerry</t>
+          <t>Amkor Technology</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GameStop</t>
+          <t>Air Lease Corporation</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AMC Entertainment</t>
+          <t>Baozun</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Koss Corporation</t>
+          <t>Qurate Retail</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Express</t>
+          <t>Guess</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Naked Brand Group</t>
+          <t>UniFirst</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sundial Growers</t>
+          <t>Commvault Systems</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ebang International</t>
+          <t>Prudental Financial</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Invest wisely, don't pour all your capital into a single economic sector. Diversification is important.</t>
+          <t>Understanding and using eToro's CopyTrader feature wisely</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: Nombres dinámicos de solapas, correcciónd de datos duplicados
</commit_message>
<xml_diff>
--- a/actions.xlsx
+++ b/actions.xlsx
@@ -484,56 +484,56 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Amazon</t>
+          <t>Microsoft</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Microsoft</t>
+          <t>Amazon</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>Nvidia</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Alibaba</t>
+          <t>Zoom</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Facebook</t>
+          <t>Paypal</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Berkshire Hathaway</t>
+          <t>Netflix</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Johnson &amp; Johnson</t>
+          <t>Facebook</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Diversify your portfolio</t>
+          <t>Use Stop Loss and Take Profit to manage your risks</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,147 +566,161 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PennyMac Financial Services</t>
+          <t>Sundial Growers</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Amkor Technology</t>
+          <t>Zomedica</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Air Lease Corporation</t>
+          <t>Check-Cap</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Baozun</t>
+          <t>Castor Maritime</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Qurate Retail</t>
+          <t>Cinedigm</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Guess</t>
+          <t>Atossa Therapeutics</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>UniFirst</t>
+          <t>Ocugen</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Commvault Systems</t>
+          <t>Fourth Wave Energy</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Prudental Financial</t>
+          <t>AbCellera Biologics</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Understanding and using eToro's CopyTrader feature wisely</t>
+          <t>Clean Energy Fuels</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Top 10 acciones a bajo costo con potencial </t>
+          <t>Invest in a diverse set of assets to spread risk</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PennyMac Financial Services</t>
+          <t xml:space="preserve">Top 10 acciones a bajo costo con potencial </t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Amkor Technology</t>
+          <t>Sundial Growers</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Air Lease Corporation</t>
+          <t>Zomedica</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Baozun</t>
+          <t>Check-Cap</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Qurate Retail</t>
+          <t>Castor Maritime</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Guess</t>
+          <t>Cinedigm</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>UniFirst</t>
+          <t>Atossa Therapeutics</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Commvault Systems</t>
+          <t>Ocugen</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Prudental Financial</t>
+          <t>Fourth Wave Energy</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Understanding and using eToro's CopyTrader feature wisely</t>
+          <t>AbCellera Biologics</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Clean Energy Fuels</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Invest in a diverse set of assets to spread risk</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: print price each symbol
</commit_message>
<xml_diff>
--- a/actions.xlsx
+++ b/actions.xlsx
@@ -7,10 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Totales" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acciones invertidas" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 empresas del momento" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 acciones bajas" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 acciones del momento" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top 10 a bajo costo" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acciones invertidas" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,19 +415,193 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Top 10 acciones del momento</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tesla</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Alphabet</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Microsoft</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Facebook</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Alibaba</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Johnson &amp; Johnson</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>UnitedHealth</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Procter &amp; Gamble</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Use stop loss and take profit orders to manage risk.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Top 10 a bajo costo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Zomedica</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Boxlight</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Castor Maritime</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Jaguar Health</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Zynga</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Aemetis</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Designer Brands</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Microvision</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Always set a stop loss to limit potential losses</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -444,287 +617,4 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Top 10 empresas del momento</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Tesla</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Apple</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Microsoft</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Amazon</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Nvidia</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Zoom</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Paypal</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Netflix</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Facebook</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Use Stop Loss and Take Profit to manage your risks</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Top 10 acciones a bajo costo con potencial </t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Sundial Growers</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Zomedica</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Check-Cap</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Castor Maritime</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Cinedigm</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Atossa Therapeutics</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Ocugen</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Fourth Wave Energy</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>AbCellera Biologics</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Clean Energy Fuels</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Invest in a diverse set of assets to spread risk</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Top 10 acciones a bajo costo con potencial </t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Sundial Growers</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Zomedica</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Check-Cap</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Castor Maritime</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Cinedigm</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Atossa Therapeutics</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Ocugen</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Fourth Wave Energy</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>AbCellera Biologics</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Clean Energy Fuels</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Invest in a diverse set of assets to spread risk</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>